<commit_message>
Data of the coupled network of Test System 2
</commit_message>
<xml_diff>
--- a/2.2. test system 2.xlsx
+++ b/2.2. test system 2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AppData\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\GithubClone\supplementary-file-for-low-carbon-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698BB78A-CA72-47E0-A5C2-3687E89AAAD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32B3489-9D69-45EF-BB1D-95F276FED3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="35216" windowHeight="19203" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TN params" sheetId="1" r:id="rId1"/>
@@ -484,9 +484,9 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -500,7 +500,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -535,7 +535,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -571,7 +571,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -607,7 +607,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -643,7 +643,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -679,7 +679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -715,7 +715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -751,7 +751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -787,7 +787,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -823,7 +823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -838,7 +838,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -853,7 +853,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -868,7 +868,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -883,7 +883,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -898,7 +898,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -913,7 +913,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -928,7 +928,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -943,7 +943,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -958,7 +958,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -973,7 +973,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -988,7 +988,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
@@ -1288,13 +1288,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E106904F-8955-43C1-A89B-D5C0923EBBD3}">
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="Q136" sqref="Q136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1315,7 +1315,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>1.071074E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>9.8181799999999997E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>1.3388429999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>4.4628100000000002E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>4.4628100000000002E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>1.0330579999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>1.1570249999999999E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>5.2066120000000002E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>1.1107438000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1865,7 +1865,7 @@
         <v>6.5206609999999996E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>2.5867768999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1965,7 +1965,7 @@
         <v>1.2495868E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2015,7 +2015,7 @@
         <v>9.7520660000000002E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>3.7190080000000002E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>1.4876033E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>1.4132231E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>2.3553719000000001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>1.5289255999999999E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>1.6198346999999998E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>1.5619835E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>6.5206609999999996E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>5.9752066E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>1.1140496E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>8.5950409999999994E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>1.107438E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>1.107438E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>2.4462809999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>2.2809919999999999E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>2.2859503999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>2.0082645E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2915,7 +2915,7 @@
         <v>4.4628100000000002E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>1.9338843000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>1.9338843000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>1.338843E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>2.1570248E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>8.1818180000000004E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>1.6033057999999999E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>1.6033057999999999E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3315,7 +3315,7 @@
         <v>1.6033057999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>1.2396694E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>7.0247933999999998E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>2.0132231E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>8.0330579999999992E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>1.0090909E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>1.4702478999999999E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>1.1429752E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -3715,7 +3715,7 @@
         <v>6.5206609999999996E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>8.157025E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>8.157025E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>1.3066115999999999E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>6.5206609999999996E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>1.2049587E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4015,7 +4015,7 @@
         <v>1.2049587E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>1.1652892999999999E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4115,7 +4115,7 @@
         <v>1.2074379999999999E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4165,7 +4165,7 @@
         <v>1.2074379999999999E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4215,7 +4215,7 @@
         <v>4.5132231000000002E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4265,7 +4265,7 @@
         <v>1.0066116E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>1.0066116E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -4365,7 +4365,7 @@
         <v>6.1735540000000004E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>7.3735537000000004E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>3.4545449999999998E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -4515,7 +4515,7 @@
         <v>1.6661156999999999E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -4565,7 +4565,7 @@
         <v>7.5867770000000003E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>6.2727269999999996E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>1.1404958999999999E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>2.7297521000000002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>1.2074379999999999E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>6.2892561999999999E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -4865,7 +4865,7 @@
         <v>4.9586780000000002E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>9.0247929999999997E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>9.0247929999999997E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5015,7 +5015,7 @@
         <v>1.1900826E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5065,7 +5065,7 @@
         <v>6.9421489999999999E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>1.4652893E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>3.7438020000000001E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>3.0471074000000001E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>1.0140496000000001E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>1.0140496000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5365,7 +5365,7 @@
         <v>1.1487603000000001E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5415,7 +5415,7 @@
         <v>1.2231405000000001E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -5465,7 +5465,7 @@
         <v>1.0578512E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -5515,7 +5515,7 @@
         <v>8.7603309999999997E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>1.2231405000000001E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -5615,7 +5615,7 @@
         <v>1.5041321999999999E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -5665,7 +5665,7 @@
         <v>1.9008264E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -5715,7 +5715,7 @@
         <v>3.2479339000000003E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>1.9933883999999999E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>1.0140496000000001E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -5865,7 +5865,7 @@
         <v>1.0140496000000001E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -5915,7 +5915,7 @@
         <v>1.0140496000000001E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -5965,7 +5965,7 @@
         <v>1.0140496000000001E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -6015,7 +6015,7 @@
         <v>9.5041320000000002E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>1.1404958999999999E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>1.4876033E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>1.4876033E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -6215,7 +6215,7 @@
         <v>1.0082644999999999E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>2.6280992E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>2.1900829999999998E-3</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>1.9338843000000001E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>7.3388430000000003E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -6465,7 +6465,7 @@
         <v>9.9421490000000008E-3</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -6515,7 +6515,7 @@
         <v>1.3289255999999999E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -6565,7 +6565,7 @@
         <v>4.8595039999999997E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>8.1818180000000004E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -6665,7 +6665,7 @@
         <v>4.6363639999999996E-3</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -6715,7 +6715,7 @@
         <v>1.1355372000000001E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>4.8347110000000002E-3</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>1.1355372000000001E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -6865,7 +6865,7 @@
         <v>7.2644629999999996E-3</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>6.2231400000000003E-3</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>6.8429750000000003E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>1.814876E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>1.0495868E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -7115,7 +7115,7 @@
         <v>2.0330579000000001E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>3.0330579E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -7215,7 +7215,7 @@
         <v>3.6198346999999999E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -7253,7 +7253,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
Data of the coupled networks of Test System 2
</commit_message>
<xml_diff>
--- a/2.2. test system 2.xlsx
+++ b/2.2. test system 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\GithubClone\supplementary-file-for-low-carbon-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32B3489-9D69-45EF-BB1D-95F276FED3DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E393BC-5B71-4104-B8B7-F1DFEBB74A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="35216" windowHeight="19203" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5778" yWindow="6398" windowWidth="26248" windowHeight="13953" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TN params" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Link</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,6 +147,10 @@
   </si>
   <si>
     <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1289,7 +1293,7 @@
   <dimension ref="A1:Q121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="Q136" sqref="Q136"/>
+      <selection activeCell="P121" sqref="P121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
@@ -7290,6 +7294,9 @@
       <c r="L121" t="s">
         <v>30</v>
       </c>
+      <c r="P121" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>